<commit_message>
Add lesional data correlations to spreadsheet.
</commit_message>
<xml_diff>
--- a/Correlation-Analysis/attributeCorrelations.xlsx
+++ b/Correlation-Analysis/attributeCorrelations.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="PMCC - AD Only" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="PMCC - Combined" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Spearman Rank - AD Only" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Spearman Rank - Combined" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="PMCC - AD Non Lesional" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="PMCC - Combined Non Lesional" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Spearman Rank - AD Non Lesional" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Spearman Rank - Combined Non Lesional" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="PMCC - AD Lesional" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Spearman Rank - AD Lesional" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,9 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="38">
   <si>
-    <t xml:space="preserve">PMCC - Combined non lesional</t>
+    <t xml:space="preserve">PMCC – AD non lesional</t>
   </si>
   <si>
     <t xml:space="preserve">ObjectiveSCORAD</t>
@@ -124,10 +126,19 @@
     <t xml:space="preserve">TNF__</t>
   </si>
   <si>
+    <t xml:space="preserve">PMCC - Combined non lesional</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spearman Rank - AD non lesional</t>
   </si>
   <si>
     <t xml:space="preserve">Spearman Rank - Combined non lesional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMCC – AD Lesional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spearman Rank – AD Lesional</t>
   </si>
 </sst>
 </file>
@@ -239,17 +250,17 @@
   </sheetPr>
   <dimension ref="A1:AG35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="33" min="5" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="33" min="5" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2110,19 +2121,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="33" min="8" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="33" min="8" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3977,17 +3988,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="33" min="5" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="33" min="5" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -5807,17 +5818,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="33" min="5" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="33" min="5" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -7657,4 +7668,3734 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AG35"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V7" activeCellId="0" sqref="V7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="33" min="5" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.38125</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.95004</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>-0.26669</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.4523</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>-0.11266</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.52372</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>-0.034904</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.68237</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.49913</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0.38864</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>-0.19967</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>-0.52333</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>-0.40252</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>-0.068754</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>-0.20106</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0.26234</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>0.46722</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>-0.26586</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>-0.31565</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>0.40786</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0.068142</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>-0.086933</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>-0.32258</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>-0.23899</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>-0.037322</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>0.047866</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <v>-0.41339</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <v>-0.32627</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <v>0.099831</v>
+      </c>
+      <c r="AF4" s="0" t="n">
+        <v>-0.0032374</v>
+      </c>
+      <c r="AG4" s="0" t="n">
+        <v>-0.11319</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.65075</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>-0.32129</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.41485</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>-0.34811</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.29471</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.21577</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.61385</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.48669</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.36043</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0.17138</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>-0.52281</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>-0.39435</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0.23315</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.12605</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0.17898</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0.24434</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>-0.14531</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>-0.37793</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>0.23801</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0.23998</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>-0.050279</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>-0.25495</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>-0.1111</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>-0.027279</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>0.18402</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>0.037889</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <v>-0.011737</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <v>-0.085902</v>
+      </c>
+      <c r="AF5" s="0" t="n">
+        <v>0.19686</v>
+      </c>
+      <c r="AG5" s="0" t="n">
+        <v>0.023135</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>-0.32751</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.51155</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>-0.21006</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.52965</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.044177</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.76769</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.57426</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0.44089</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>-0.10613</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>-0.60634</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>-0.46374</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>0.022245</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>-0.12258</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0.2759</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>0.46623</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>-0.26742</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>-0.38685</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>0.41535</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0.13699</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>-0.088376</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>-0.35102</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>-0.2338</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>-0.039863</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>0.10144</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <v>-0.32674</v>
+      </c>
+      <c r="AD6" s="0" t="n">
+        <v>-0.27194</v>
+      </c>
+      <c r="AE6" s="0" t="n">
+        <v>0.052992</v>
+      </c>
+      <c r="AF6" s="0" t="n">
+        <v>0.063803</v>
+      </c>
+      <c r="AG6" s="0" t="n">
+        <v>-0.085156</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>-0.38335</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.38883</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>-0.44744</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.11557</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>-0.30653</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>-0.42088</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>-0.27482</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>-0.197</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0.46851</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>-0.10077</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>-0.48466</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.12373</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0.039185</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>-0.60071</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>0.054941</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>0.20249</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>-0.73902</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0.26768</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>0.14053</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>0.38426</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>0.19349</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>0.091939</v>
+      </c>
+      <c r="AB7" s="0" t="n">
+        <v>-0.19622</v>
+      </c>
+      <c r="AC7" s="0" t="n">
+        <v>0.35745</v>
+      </c>
+      <c r="AD7" s="0" t="n">
+        <v>-0.086139</v>
+      </c>
+      <c r="AE7" s="0" t="n">
+        <v>-0.041639</v>
+      </c>
+      <c r="AF7" s="0" t="n">
+        <v>0.053562</v>
+      </c>
+      <c r="AG7" s="0" t="n">
+        <v>0.070627</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>-0.17077</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.64385</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.098171</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.46731</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.50229</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0.64667</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>0.044274</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>-0.37993</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>-0.30953</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>0.2428</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>-0.1537</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0.13462</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>0.21757</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>-0.13118</v>
+      </c>
+      <c r="U8" s="0" t="n">
+        <v>-0.12051</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <v>0.36403</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>0.13359</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <v>0.23653</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>0.0084043</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <v>-0.47181</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <v>-0.046618</v>
+      </c>
+      <c r="AB8" s="0" t="n">
+        <v>-0.13738</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <v>-0.37426</v>
+      </c>
+      <c r="AD8" s="0" t="n">
+        <v>0.0016594</v>
+      </c>
+      <c r="AE8" s="0" t="n">
+        <v>0.10977</v>
+      </c>
+      <c r="AF8" s="0" t="n">
+        <v>0.096063</v>
+      </c>
+      <c r="AG8" s="0" t="n">
+        <v>-0.51</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>-0.023608</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>-0.02053</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>-0.38602</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.095338</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0.18342</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>-0.34258</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0.20062</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>0.25057</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>-0.32459</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>-0.10304</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>-0.15355</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>-0.52232</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>-0.32652</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <v>0.23165</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <v>-0.19837</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0.35731</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>0.30919</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>0.24772</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>0.15151</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <v>0.26193</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <v>-0.11342</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <v>0.23933</v>
+      </c>
+      <c r="AD9" s="0" t="n">
+        <v>0.30067</v>
+      </c>
+      <c r="AE9" s="0" t="n">
+        <v>0.37991</v>
+      </c>
+      <c r="AF9" s="0" t="n">
+        <v>-0.13167</v>
+      </c>
+      <c r="AG9" s="0" t="n">
+        <v>-0.13163</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.2466</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.49746</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.71256</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>0.5699</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>-0.14532</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>-0.4567</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>-0.06762</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>0.29658</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>-0.21418</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0.14643</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>0.46202</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>0.098905</v>
+      </c>
+      <c r="U10" s="0" t="n">
+        <v>-0.17655</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>0.5412</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>0.20174</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>0.063841</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>-0.055758</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>-0.24897</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <v>0.014321</v>
+      </c>
+      <c r="AB10" s="0" t="n">
+        <v>0.11352</v>
+      </c>
+      <c r="AC10" s="0" t="n">
+        <v>-0.50558</v>
+      </c>
+      <c r="AD10" s="0" t="n">
+        <v>0.013698</v>
+      </c>
+      <c r="AE10" s="0" t="n">
+        <v>0.1006</v>
+      </c>
+      <c r="AF10" s="0" t="n">
+        <v>-0.10315</v>
+      </c>
+      <c r="AG10" s="0" t="n">
+        <v>-0.22384</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0.18094</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.15946</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>0.080096</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>-0.10509</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>-0.13681</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>0.11615</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.052812</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0.32797</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>-0.028046</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>0.024485</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <v>0.1366</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <v>-0.31723</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>0.34825</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <v>0.087271</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>0.38141</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <v>0.13867</v>
+      </c>
+      <c r="AA11" s="0" t="n">
+        <v>0.18283</v>
+      </c>
+      <c r="AB11" s="0" t="n">
+        <v>0.20778</v>
+      </c>
+      <c r="AC11" s="0" t="n">
+        <v>0.22161</v>
+      </c>
+      <c r="AD11" s="0" t="n">
+        <v>0.14727</v>
+      </c>
+      <c r="AE11" s="0" t="n">
+        <v>-0.013475</v>
+      </c>
+      <c r="AF11" s="0" t="n">
+        <v>0.17545</v>
+      </c>
+      <c r="AG11" s="0" t="n">
+        <v>0.29256</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.4257</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>0.32179</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>0.053487</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>-0.65254</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>-0.25385</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>0.4146</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.091924</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0.1562</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>0.53065</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>-0.13653</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>-0.23849</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>0.28332</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>-0.082361</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <v>0.10975</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <v>-0.37637</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>-0.30992</v>
+      </c>
+      <c r="AA12" s="0" t="n">
+        <v>-0.023076</v>
+      </c>
+      <c r="AB12" s="0" t="n">
+        <v>0.36146</v>
+      </c>
+      <c r="AC12" s="0" t="n">
+        <v>-0.16921</v>
+      </c>
+      <c r="AD12" s="0" t="n">
+        <v>-0.23244</v>
+      </c>
+      <c r="AE12" s="0" t="n">
+        <v>0.19058</v>
+      </c>
+      <c r="AF12" s="0" t="n">
+        <v>0.027771</v>
+      </c>
+      <c r="AG12" s="0" t="n">
+        <v>0.095771</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>0.69275</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>-0.078927</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>-0.37208</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>-0.26305</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>0.3093</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>-0.18553</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>0.15758</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>0.21901</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>-0.21875</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <v>-0.012664</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>0.48377</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>0.18228</v>
+      </c>
+      <c r="X13" s="0" t="n">
+        <v>-0.041571</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>-0.039139</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>-0.10303</v>
+      </c>
+      <c r="AA13" s="0" t="n">
+        <v>-0.061688</v>
+      </c>
+      <c r="AB13" s="0" t="n">
+        <v>0.10711</v>
+      </c>
+      <c r="AC13" s="0" t="n">
+        <v>-0.092859</v>
+      </c>
+      <c r="AD13" s="0" t="n">
+        <v>0.10208</v>
+      </c>
+      <c r="AE13" s="0" t="n">
+        <v>0.051377</v>
+      </c>
+      <c r="AF13" s="0" t="n">
+        <v>-0.058832</v>
+      </c>
+      <c r="AG13" s="0" t="n">
+        <v>-0.26851</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>-0.0010102</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>-0.4423</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>-0.29546</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>0.15919</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>-0.40362</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>0.004966</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>-0.098989</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>-0.25353</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <v>-0.044896</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>0.38421</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>0.26888</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>0.20931</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>0.11798</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <v>-0.46488</v>
+      </c>
+      <c r="AA14" s="0" t="n">
+        <v>-0.043616</v>
+      </c>
+      <c r="AB14" s="0" t="n">
+        <v>0.13694</v>
+      </c>
+      <c r="AC14" s="0" t="n">
+        <v>-0.1548</v>
+      </c>
+      <c r="AD14" s="0" t="n">
+        <v>0.091268</v>
+      </c>
+      <c r="AE14" s="0" t="n">
+        <v>0.16592</v>
+      </c>
+      <c r="AF14" s="0" t="n">
+        <v>-0.020225</v>
+      </c>
+      <c r="AG14" s="0" t="n">
+        <v>-0.42142</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>0.098955</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>-0.11313</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>0.13515</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>-0.031745</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>-0.24922</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>0.075613</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>0.24303</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>0.088717</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <v>0.073127</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>0.13841</v>
+      </c>
+      <c r="X15" s="0" t="n">
+        <v>-0.16562</v>
+      </c>
+      <c r="Y15" s="0" t="n">
+        <v>-0.038283</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <v>0.062089</v>
+      </c>
+      <c r="AA15" s="0" t="n">
+        <v>-0.014168</v>
+      </c>
+      <c r="AB15" s="0" t="n">
+        <v>-0.069503</v>
+      </c>
+      <c r="AC15" s="0" t="n">
+        <v>0.26535</v>
+      </c>
+      <c r="AD15" s="0" t="n">
+        <v>0.15817</v>
+      </c>
+      <c r="AE15" s="0" t="n">
+        <v>-0.175</v>
+      </c>
+      <c r="AF15" s="0" t="n">
+        <v>0.065294</v>
+      </c>
+      <c r="AG15" s="0" t="n">
+        <v>0.13769</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>0.24509</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>-0.28352</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>0.11816</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>-0.15676</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>-0.44711</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>0.27215</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>0.39799</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>-0.42718</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>-0.090247</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <v>0.060937</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <v>0.35289</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <v>0.28497</v>
+      </c>
+      <c r="AA16" s="0" t="n">
+        <v>-0.044073</v>
+      </c>
+      <c r="AB16" s="0" t="n">
+        <v>-0.34946</v>
+      </c>
+      <c r="AC16" s="0" t="n">
+        <v>0.18214</v>
+      </c>
+      <c r="AD16" s="0" t="n">
+        <v>0.12023</v>
+      </c>
+      <c r="AE16" s="0" t="n">
+        <v>-0.024239</v>
+      </c>
+      <c r="AF16" s="0" t="n">
+        <v>0.05936</v>
+      </c>
+      <c r="AG16" s="0" t="n">
+        <v>-0.080893</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>0.26465</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0.31464</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>-0.25339</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>-0.086536</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>-0.043425</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>0.27119</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>-0.036995</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>-0.35802</v>
+      </c>
+      <c r="X17" s="0" t="n">
+        <v>0.019717</v>
+      </c>
+      <c r="Y17" s="0" t="n">
+        <v>-0.22837</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <v>0.00017265</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <v>0.22937</v>
+      </c>
+      <c r="AB17" s="0" t="n">
+        <v>0.16964</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <v>-0.040392</v>
+      </c>
+      <c r="AD17" s="0" t="n">
+        <v>0.37656</v>
+      </c>
+      <c r="AE17" s="0" t="n">
+        <v>0.15573</v>
+      </c>
+      <c r="AF17" s="0" t="n">
+        <v>0.068552</v>
+      </c>
+      <c r="AG17" s="0" t="n">
+        <v>0.30735</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>0.18631</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>0.0087967</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <v>0.23307</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>0.066299</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>0.27861</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>0.25809</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>-0.21391</v>
+      </c>
+      <c r="X18" s="0" t="n">
+        <v>0.14617</v>
+      </c>
+      <c r="Y18" s="0" t="n">
+        <v>-0.099455</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <v>-0.10492</v>
+      </c>
+      <c r="AA18" s="0" t="n">
+        <v>0.059615</v>
+      </c>
+      <c r="AB18" s="0" t="n">
+        <v>0.43727</v>
+      </c>
+      <c r="AC18" s="0" t="n">
+        <v>0.0054759</v>
+      </c>
+      <c r="AD18" s="0" t="n">
+        <v>0.16736</v>
+      </c>
+      <c r="AE18" s="0" t="n">
+        <v>0.14044</v>
+      </c>
+      <c r="AF18" s="0" t="n">
+        <v>0.057682</v>
+      </c>
+      <c r="AG18" s="0" t="n">
+        <v>-0.061206</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>-0.0051867</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <v>-0.11766</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>-0.13714</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>0.012547</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <v>-0.28081</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>-0.35044</v>
+      </c>
+      <c r="X19" s="0" t="n">
+        <v>0.24878</v>
+      </c>
+      <c r="Y19" s="0" t="n">
+        <v>-0.13926</v>
+      </c>
+      <c r="Z19" s="0" t="n">
+        <v>0.0030104</v>
+      </c>
+      <c r="AA19" s="0" t="n">
+        <v>-0.11615</v>
+      </c>
+      <c r="AB19" s="0" t="n">
+        <v>-0.17794</v>
+      </c>
+      <c r="AC19" s="0" t="n">
+        <v>0.1383</v>
+      </c>
+      <c r="AD19" s="0" t="n">
+        <v>-0.27199</v>
+      </c>
+      <c r="AE19" s="0" t="n">
+        <v>0.1317</v>
+      </c>
+      <c r="AF19" s="0" t="n">
+        <v>0.062507</v>
+      </c>
+      <c r="AG19" s="0" t="n">
+        <v>0.23625</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>0.013731</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>0.21472</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>-0.11662</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <v>0.10116</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>0.18023</v>
+      </c>
+      <c r="X20" s="0" t="n">
+        <v>-0.020152</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <v>0.2519</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <v>0.012684</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <v>-0.17107</v>
+      </c>
+      <c r="AB20" s="0" t="n">
+        <v>-0.18873</v>
+      </c>
+      <c r="AC20" s="0" t="n">
+        <v>-0.015613</v>
+      </c>
+      <c r="AD20" s="0" t="n">
+        <v>-0.47382</v>
+      </c>
+      <c r="AE20" s="0" t="n">
+        <v>-0.079926</v>
+      </c>
+      <c r="AF20" s="0" t="n">
+        <v>0.12419</v>
+      </c>
+      <c r="AG20" s="0" t="n">
+        <v>-0.058631</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>0.16457</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>-0.18851</v>
+      </c>
+      <c r="V21" s="0" t="n">
+        <v>0.45458</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>-0.2985</v>
+      </c>
+      <c r="X21" s="0" t="n">
+        <v>-0.37291</v>
+      </c>
+      <c r="Y21" s="0" t="n">
+        <v>-0.4375</v>
+      </c>
+      <c r="Z21" s="0" t="n">
+        <v>0.12266</v>
+      </c>
+      <c r="AA21" s="0" t="n">
+        <v>-0.23012</v>
+      </c>
+      <c r="AB21" s="0" t="n">
+        <v>0.041763</v>
+      </c>
+      <c r="AC21" s="0" t="n">
+        <v>-0.44534</v>
+      </c>
+      <c r="AD21" s="0" t="n">
+        <v>-0.17585</v>
+      </c>
+      <c r="AE21" s="0" t="n">
+        <v>-0.22614</v>
+      </c>
+      <c r="AF21" s="0" t="n">
+        <v>-0.057419</v>
+      </c>
+      <c r="AG21" s="0" t="n">
+        <v>0.069868</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <v>-0.086329</v>
+      </c>
+      <c r="V22" s="0" t="n">
+        <v>0.15537</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <v>0.12329</v>
+      </c>
+      <c r="X22" s="0" t="n">
+        <v>0.046534</v>
+      </c>
+      <c r="Y22" s="0" t="n">
+        <v>0.13074</v>
+      </c>
+      <c r="Z22" s="0" t="n">
+        <v>0.27625</v>
+      </c>
+      <c r="AA22" s="0" t="n">
+        <v>-0.28554</v>
+      </c>
+      <c r="AB22" s="0" t="n">
+        <v>-0.24205</v>
+      </c>
+      <c r="AC22" s="0" t="n">
+        <v>-0.27901</v>
+      </c>
+      <c r="AD22" s="0" t="n">
+        <v>-0.25875</v>
+      </c>
+      <c r="AE22" s="0" t="n">
+        <v>-0.29157</v>
+      </c>
+      <c r="AF22" s="0" t="n">
+        <v>-0.080083</v>
+      </c>
+      <c r="AG22" s="0" t="n">
+        <v>-0.0089048</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V23" s="0" t="n">
+        <v>-0.49291</v>
+      </c>
+      <c r="W23" s="0" t="n">
+        <v>-0.14104</v>
+      </c>
+      <c r="X23" s="0" t="n">
+        <v>-0.0074411</v>
+      </c>
+      <c r="Y23" s="0" t="n">
+        <v>0.2917</v>
+      </c>
+      <c r="Z23" s="0" t="n">
+        <v>0.30195</v>
+      </c>
+      <c r="AA23" s="0" t="n">
+        <v>-0.018929</v>
+      </c>
+      <c r="AB23" s="0" t="n">
+        <v>-0.019692</v>
+      </c>
+      <c r="AC23" s="0" t="n">
+        <v>0.17604</v>
+      </c>
+      <c r="AD23" s="0" t="n">
+        <v>0.24757</v>
+      </c>
+      <c r="AE23" s="0" t="n">
+        <v>-0.15189</v>
+      </c>
+      <c r="AF23" s="0" t="n">
+        <v>0.27147</v>
+      </c>
+      <c r="AG23" s="0" t="n">
+        <v>-0.057034</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W24" s="0" t="n">
+        <v>-0.027811</v>
+      </c>
+      <c r="X24" s="0" t="n">
+        <v>-0.062544</v>
+      </c>
+      <c r="Y24" s="0" t="n">
+        <v>-0.2536</v>
+      </c>
+      <c r="Z24" s="0" t="n">
+        <v>-0.33927</v>
+      </c>
+      <c r="AA24" s="0" t="n">
+        <v>-0.25553</v>
+      </c>
+      <c r="AB24" s="0" t="n">
+        <v>0.024192</v>
+      </c>
+      <c r="AC24" s="0" t="n">
+        <v>-0.40079</v>
+      </c>
+      <c r="AD24" s="0" t="n">
+        <v>-0.096742</v>
+      </c>
+      <c r="AE24" s="0" t="n">
+        <v>0.16421</v>
+      </c>
+      <c r="AF24" s="0" t="n">
+        <v>-0.19733</v>
+      </c>
+      <c r="AG24" s="0" t="n">
+        <v>-0.32991</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X25" s="0" t="n">
+        <v>-0.025638</v>
+      </c>
+      <c r="Y25" s="0" t="n">
+        <v>0.31251</v>
+      </c>
+      <c r="Z25" s="0" t="n">
+        <v>0.057675</v>
+      </c>
+      <c r="AA25" s="0" t="n">
+        <v>0.40372</v>
+      </c>
+      <c r="AB25" s="0" t="n">
+        <v>0.0075805</v>
+      </c>
+      <c r="AC25" s="0" t="n">
+        <v>0.26554</v>
+      </c>
+      <c r="AD25" s="0" t="n">
+        <v>0.2171</v>
+      </c>
+      <c r="AE25" s="0" t="n">
+        <v>0.0093065</v>
+      </c>
+      <c r="AF25" s="0" t="n">
+        <v>-0.11858</v>
+      </c>
+      <c r="AG25" s="0" t="n">
+        <v>-0.052554</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y26" s="0" t="n">
+        <v>0.18484</v>
+      </c>
+      <c r="Z26" s="0" t="n">
+        <v>-0.18701</v>
+      </c>
+      <c r="AA26" s="0" t="n">
+        <v>-0.081227</v>
+      </c>
+      <c r="AB26" s="0" t="n">
+        <v>-0.02279</v>
+      </c>
+      <c r="AC26" s="0" t="n">
+        <v>-0.091312</v>
+      </c>
+      <c r="AD26" s="0" t="n">
+        <v>-0.10843</v>
+      </c>
+      <c r="AE26" s="0" t="n">
+        <v>0.62782</v>
+      </c>
+      <c r="AF26" s="0" t="n">
+        <v>0.08595</v>
+      </c>
+      <c r="AG26" s="0" t="n">
+        <v>-0.28221</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z27" s="0" t="n">
+        <v>-0.076754</v>
+      </c>
+      <c r="AA27" s="0" t="n">
+        <v>-0.17872</v>
+      </c>
+      <c r="AB27" s="0" t="n">
+        <v>-0.15031</v>
+      </c>
+      <c r="AC27" s="0" t="n">
+        <v>0.18379</v>
+      </c>
+      <c r="AD27" s="0" t="n">
+        <v>-0.14503</v>
+      </c>
+      <c r="AE27" s="0" t="n">
+        <v>0.2129</v>
+      </c>
+      <c r="AF27" s="0" t="n">
+        <v>-0.052469</v>
+      </c>
+      <c r="AG27" s="0" t="n">
+        <v>-0.46789</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA28" s="0" t="n">
+        <v>0.010511</v>
+      </c>
+      <c r="AB28" s="0" t="n">
+        <v>-0.27819</v>
+      </c>
+      <c r="AC28" s="0" t="n">
+        <v>0.17927</v>
+      </c>
+      <c r="AD28" s="0" t="n">
+        <v>0.15556</v>
+      </c>
+      <c r="AE28" s="0" t="n">
+        <v>-0.45551</v>
+      </c>
+      <c r="AF28" s="0" t="n">
+        <v>0.1476</v>
+      </c>
+      <c r="AG28" s="0" t="n">
+        <v>0.22647</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB29" s="0" t="n">
+        <v>0.44198</v>
+      </c>
+      <c r="AC29" s="0" t="n">
+        <v>0.30569</v>
+      </c>
+      <c r="AD29" s="0" t="n">
+        <v>0.55903</v>
+      </c>
+      <c r="AE29" s="0" t="n">
+        <v>0.22671</v>
+      </c>
+      <c r="AF29" s="0" t="n">
+        <v>-0.038898</v>
+      </c>
+      <c r="AG29" s="0" t="n">
+        <v>0.37725</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC30" s="0" t="n">
+        <v>0.15648</v>
+      </c>
+      <c r="AD30" s="0" t="n">
+        <v>0.37504</v>
+      </c>
+      <c r="AE30" s="0" t="n">
+        <v>0.26391</v>
+      </c>
+      <c r="AF30" s="0" t="n">
+        <v>-0.050487</v>
+      </c>
+      <c r="AG30" s="0" t="n">
+        <v>0.39661</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD31" s="0" t="n">
+        <v>0.29218</v>
+      </c>
+      <c r="AE31" s="0" t="n">
+        <v>0.09616</v>
+      </c>
+      <c r="AF31" s="0" t="n">
+        <v>-0.15155</v>
+      </c>
+      <c r="AG31" s="0" t="n">
+        <v>0.23387</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE32" s="0" t="n">
+        <v>-0.037894</v>
+      </c>
+      <c r="AF32" s="0" t="n">
+        <v>0.22945</v>
+      </c>
+      <c r="AG32" s="0" t="n">
+        <v>0.15033</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF33" s="0" t="n">
+        <v>-0.14971</v>
+      </c>
+      <c r="AG33" s="0" t="n">
+        <v>-0.25182</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG34" s="0" t="n">
+        <v>-0.095382</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AG1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E4:AG33">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AG35"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N59" activeCellId="0" sqref="N59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="33" min="5" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.4715</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.91562</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>-0.31187</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.62288</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>-0.11353</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.57416</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>-0.024364</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.60083</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.56242</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0.39017</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>-0.32543</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>-0.45455</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>-0.30013</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>-0.20492</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>-0.30361</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0.24097</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>0.43671</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>-0.36451</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>-0.53264</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>0.53328</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0.047412</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>0.033493</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>-0.55514</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>-0.38808</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>-0.10135</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>-0.098782</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <v>-0.39896</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <v>-0.23923</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <v>0.077425</v>
+      </c>
+      <c r="AF4" s="0" t="n">
+        <v>-0.12486</v>
+      </c>
+      <c r="AG4" s="0" t="n">
+        <v>-0.10831</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.7505</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>-0.22965</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.30474</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>-0.37197</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.27374</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.11594</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.49782</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.34578</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.22048</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0.037118</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>-0.48898</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>-0.54093</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>-0.10349</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>-0.045842</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0.05894</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0.19385</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>-0.27025</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>-0.49596</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>0.21699</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0.20563</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>-0.11351</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>-0.48472</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>-0.18756</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>-0.032308</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>-0.056126</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>-0.13799</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <v>-0.044532</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <v>-0.14626</v>
+      </c>
+      <c r="AF5" s="0" t="n">
+        <v>0.041267</v>
+      </c>
+      <c r="AG5" s="0" t="n">
+        <v>-0.047588</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>-0.29304</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.60261</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>-0.22435</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.48957</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.073929</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.64188</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.52696</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0.31043</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>-0.18352</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>-0.51043</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>-0.47478</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>-0.16873</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>-0.26435</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0.24087</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>0.37478</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>-0.34348</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>-0.55415</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>0.43565</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0.18609</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>-0.041739</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>-0.5636</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>-0.32442</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>-0.0078261</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>-0.066986</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <v>-0.26962</v>
+      </c>
+      <c r="AD6" s="0" t="n">
+        <v>-0.12696</v>
+      </c>
+      <c r="AE6" s="0" t="n">
+        <v>0.0086957</v>
+      </c>
+      <c r="AF6" s="0" t="n">
+        <v>-0.086106</v>
+      </c>
+      <c r="AG6" s="0" t="n">
+        <v>-0.085217</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>-0.44</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.34609</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>-0.41391</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.16569</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>-0.096108</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>-0.39391</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>-0.16917</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0.3087</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0.14174</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>0.075234</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.24348</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0.068696</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>-0.51913</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>-0.083478</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>0.30709</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>-0.74261</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0.26783</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>0.16696</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>0.4614</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>0.13786</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>0.22522</v>
+      </c>
+      <c r="AB7" s="0" t="n">
+        <v>0.26359</v>
+      </c>
+      <c r="AC7" s="0" t="n">
+        <v>0.47967</v>
+      </c>
+      <c r="AD7" s="0" t="n">
+        <v>0.086087</v>
+      </c>
+      <c r="AE7" s="0" t="n">
+        <v>0.092174</v>
+      </c>
+      <c r="AF7" s="0" t="n">
+        <v>0.18743</v>
+      </c>
+      <c r="AG7" s="0" t="n">
+        <v>0.15304</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>-0.24</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.63217</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.049141</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.39878</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.42696</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0.60783</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>0.01609</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>-0.40522</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>-0.34957</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>-0.13351</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>-0.38174</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0.30261</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>0.23217</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>-0.047826</v>
+      </c>
+      <c r="U8" s="0" t="n">
+        <v>-0.27925</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <v>0.48783</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>0.078261</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <v>0.16435</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>-0.18656</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <v>-0.56404</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <v>-0.12609</v>
+      </c>
+      <c r="AB8" s="0" t="n">
+        <v>-0.3097</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <v>-0.45619</v>
+      </c>
+      <c r="AD8" s="0" t="n">
+        <v>-0.20261</v>
+      </c>
+      <c r="AE8" s="0" t="n">
+        <v>0.16522</v>
+      </c>
+      <c r="AF8" s="0" t="n">
+        <v>-0.0039139</v>
+      </c>
+      <c r="AG8" s="0" t="n">
+        <v>-0.48261</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>-0.035652</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.066101</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>-0.28093</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.010435</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>-0.057391</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>-0.27049</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0.17043</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>0.34087</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>0.093933</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.12174</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>-0.082609</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>-0.58783</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>-0.41565</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <v>0.33841</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <v>-0.20696</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0.3913</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>0.30609</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>0.40791</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>0.20352</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <v>0.30261</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <v>0.20966</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <v>0.39139</v>
+      </c>
+      <c r="AD9" s="0" t="n">
+        <v>0.35739</v>
+      </c>
+      <c r="AE9" s="0" t="n">
+        <v>0.38348</v>
+      </c>
+      <c r="AF9" s="0" t="n">
+        <v>-0.046097</v>
+      </c>
+      <c r="AG9" s="0" t="n">
+        <v>-0.028696</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.21265</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.45532</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.78261</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>0.58348</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>-0.092629</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>-0.41826</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>-0.029565</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>0.066536</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>-0.17739</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0.17043</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>0.38696</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>-0.022609</v>
+      </c>
+      <c r="U10" s="0" t="n">
+        <v>-0.27403</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>0.50522</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>0.22522</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>0.044348</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>-0.23875</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>-0.33007</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <v>0.049565</v>
+      </c>
+      <c r="AB10" s="0" t="n">
+        <v>0.028708</v>
+      </c>
+      <c r="AC10" s="0" t="n">
+        <v>-0.31616</v>
+      </c>
+      <c r="AD10" s="0" t="n">
+        <v>-0.033913</v>
+      </c>
+      <c r="AE10" s="0" t="n">
+        <v>0.10522</v>
+      </c>
+      <c r="AF10" s="0" t="n">
+        <v>-0.15438</v>
+      </c>
+      <c r="AG10" s="0" t="n">
+        <v>-0.14609</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0.31448</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.026962</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>-0.19222</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>0.301</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>-0.013046</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>0.020004</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>0.47238</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.35399</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0.177</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>-0.021744</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>0.066101</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <v>0.29846</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <v>-0.32746</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>0.26571</v>
+      </c>
+      <c r="X11" s="0" t="n">
+        <v>0.1309</v>
+      </c>
+      <c r="Y11" s="0" t="n">
+        <v>0.3532</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <v>0.21531</v>
+      </c>
+      <c r="AA11" s="0" t="n">
+        <v>0.21831</v>
+      </c>
+      <c r="AB11" s="0" t="n">
+        <v>0.35849</v>
+      </c>
+      <c r="AC11" s="0" t="n">
+        <v>0.34841</v>
+      </c>
+      <c r="AD11" s="0" t="n">
+        <v>0.26832</v>
+      </c>
+      <c r="AE11" s="0" t="n">
+        <v>0.10828</v>
+      </c>
+      <c r="AF11" s="0" t="n">
+        <v>0.30926</v>
+      </c>
+      <c r="AG11" s="0" t="n">
+        <v>0.38748</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.42009</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>0.2918</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>0.11875</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>-0.60187</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>-0.19352</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>0.28752</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.060448</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0.049576</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>0.46314</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>-0.25658</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>-0.22493</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>0.18743</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>-0.022179</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <v>0.10089</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <v>-0.32318</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>-0.24054</v>
+      </c>
+      <c r="AA12" s="0" t="n">
+        <v>0.080887</v>
+      </c>
+      <c r="AB12" s="0" t="n">
+        <v>0.36067</v>
+      </c>
+      <c r="AC12" s="0" t="n">
+        <v>0.027403</v>
+      </c>
+      <c r="AD12" s="0" t="n">
+        <v>-0.093064</v>
+      </c>
+      <c r="AE12" s="0" t="n">
+        <v>0.19222</v>
+      </c>
+      <c r="AF12" s="0" t="n">
+        <v>0.046977</v>
+      </c>
+      <c r="AG12" s="0" t="n">
+        <v>0.177</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>0.52609</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>-0.085236</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>-0.43739</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>-0.24261</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>-0.006958</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>-0.15391</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>0.098261</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>0.34696</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>-0.07913</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <v>-0.24793</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>0.60522</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>0.20261</v>
+      </c>
+      <c r="X13" s="0" t="n">
+        <v>-0.089565</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>-0.34703</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>-0.16177</v>
+      </c>
+      <c r="AA13" s="0" t="n">
+        <v>-0.033043</v>
+      </c>
+      <c r="AB13" s="0" t="n">
+        <v>0.033058</v>
+      </c>
+      <c r="AC13" s="0" t="n">
+        <v>-0.12264</v>
+      </c>
+      <c r="AD13" s="0" t="n">
+        <v>-0.0095652</v>
+      </c>
+      <c r="AE13" s="0" t="n">
+        <v>-0.006087</v>
+      </c>
+      <c r="AF13" s="0" t="n">
+        <v>-0.40618</v>
+      </c>
+      <c r="AG13" s="0" t="n">
+        <v>-0.12609</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>-0.080452</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>-0.50783</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>-0.34696</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>-0.17873</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>-0.48</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>-0.11217</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>0.066957</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>-0.24</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <v>-0.31796</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>0.42087</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>0.095652</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>0.21739</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>-0.23092</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <v>-0.64014</v>
+      </c>
+      <c r="AA14" s="0" t="n">
+        <v>-0.14696</v>
+      </c>
+      <c r="AB14" s="0" t="n">
+        <v>-0.10048</v>
+      </c>
+      <c r="AC14" s="0" t="n">
+        <v>-0.41183</v>
+      </c>
+      <c r="AD14" s="0" t="n">
+        <v>-0.2687</v>
+      </c>
+      <c r="AE14" s="0" t="n">
+        <v>0.18609</v>
+      </c>
+      <c r="AF14" s="0" t="n">
+        <v>-0.35921</v>
+      </c>
+      <c r="AG14" s="0" t="n">
+        <v>-0.40087</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>0.13829</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>0.030876</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>0.25968</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0.058708</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>-0.25832</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>0.010002</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>0.31833</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>0.26365</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <v>0.023048</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>0.08741</v>
+      </c>
+      <c r="X15" s="0" t="n">
+        <v>-0.10089</v>
+      </c>
+      <c r="Y15" s="0" t="n">
+        <v>0.17355</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <v>0.052197</v>
+      </c>
+      <c r="AA15" s="0" t="n">
+        <v>0.040009</v>
+      </c>
+      <c r="AB15" s="0" t="n">
+        <v>0.035675</v>
+      </c>
+      <c r="AC15" s="0" t="n">
+        <v>0.13789</v>
+      </c>
+      <c r="AD15" s="0" t="n">
+        <v>0.23657</v>
+      </c>
+      <c r="AE15" s="0" t="n">
+        <v>-0.098282</v>
+      </c>
+      <c r="AF15" s="0" t="n">
+        <v>0.058721</v>
+      </c>
+      <c r="AG15" s="0" t="n">
+        <v>0.096108</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>0.3487</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>-0.03392</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>0.073043</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>-0.068696</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>-0.37565</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>0.31391</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>0.51414</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>-0.31304</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>-0.14522</v>
+      </c>
+      <c r="X16" s="0" t="n">
+        <v>0.053043</v>
+      </c>
+      <c r="Y16" s="0" t="n">
+        <v>0.47315</v>
+      </c>
+      <c r="Z16" s="0" t="n">
+        <v>0.28354</v>
+      </c>
+      <c r="AA16" s="0" t="n">
+        <v>-0.071304</v>
+      </c>
+      <c r="AB16" s="0" t="n">
+        <v>-0.057416</v>
+      </c>
+      <c r="AC16" s="0" t="n">
+        <v>0.21483</v>
+      </c>
+      <c r="AD16" s="0" t="n">
+        <v>0.27913</v>
+      </c>
+      <c r="AE16" s="0" t="n">
+        <v>-0.034783</v>
+      </c>
+      <c r="AF16" s="0" t="n">
+        <v>0.18787</v>
+      </c>
+      <c r="AG16" s="0" t="n">
+        <v>-0.013043</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>0.47097</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0.37304</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>-0.11826</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>-0.073043</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>-0.024348</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>0.35015</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>-0.11043</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>-0.20261</v>
+      </c>
+      <c r="X17" s="0" t="n">
+        <v>-0.061739</v>
+      </c>
+      <c r="Y17" s="0" t="n">
+        <v>0.26832</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <v>0.15917</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <v>0.37304</v>
+      </c>
+      <c r="AB17" s="0" t="n">
+        <v>0.35624</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <v>0.20657</v>
+      </c>
+      <c r="AD17" s="0" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="AE17" s="0" t="n">
+        <v>0.21913</v>
+      </c>
+      <c r="AF17" s="0" t="n">
+        <v>0.19309</v>
+      </c>
+      <c r="AG17" s="0" t="n">
+        <v>0.35304</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>0.45445</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>0.089585</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <v>-0.078713</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>0.020004</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>0.54383</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>-0.13264</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>-0.010872</v>
+      </c>
+      <c r="X18" s="0" t="n">
+        <v>0.064362</v>
+      </c>
+      <c r="Y18" s="0" t="n">
+        <v>0.42497</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <v>0.24184</v>
+      </c>
+      <c r="AA18" s="0" t="n">
+        <v>0.49054</v>
+      </c>
+      <c r="AB18" s="0" t="n">
+        <v>0.74918</v>
+      </c>
+      <c r="AC18" s="0" t="n">
+        <v>0.53023</v>
+      </c>
+      <c r="AD18" s="0" t="n">
+        <v>0.39487</v>
+      </c>
+      <c r="AE18" s="0" t="n">
+        <v>0.30876</v>
+      </c>
+      <c r="AF18" s="0" t="n">
+        <v>0.20313</v>
+      </c>
+      <c r="AG18" s="0" t="n">
+        <v>0.3205</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>0.071304</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <v>-0.17043</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>-0.017391</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>0.38843</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <v>-0.42261</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>-0.21913</v>
+      </c>
+      <c r="X19" s="0" t="n">
+        <v>0.24783</v>
+      </c>
+      <c r="Y19" s="0" t="n">
+        <v>0.29354</v>
+      </c>
+      <c r="Z19" s="0" t="n">
+        <v>0.31398</v>
+      </c>
+      <c r="AA19" s="0" t="n">
+        <v>0.067826</v>
+      </c>
+      <c r="AB19" s="0" t="n">
+        <v>0.19269</v>
+      </c>
+      <c r="AC19" s="0" t="n">
+        <v>0.43618</v>
+      </c>
+      <c r="AD19" s="0" t="n">
+        <v>-0.049565</v>
+      </c>
+      <c r="AE19" s="0" t="n">
+        <v>0.1687</v>
+      </c>
+      <c r="AF19" s="0" t="n">
+        <v>0.26962</v>
+      </c>
+      <c r="AG19" s="0" t="n">
+        <v>0.3687</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>-0.047826</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>0.15739</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>0.18834</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <v>0.11913</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>0.20348</v>
+      </c>
+      <c r="X20" s="0" t="n">
+        <v>-0.068696</v>
+      </c>
+      <c r="Y20" s="0" t="n">
+        <v>0.25223</v>
+      </c>
+      <c r="Z20" s="0" t="n">
+        <v>0.043923</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <v>-0.047826</v>
+      </c>
+      <c r="AB20" s="0" t="n">
+        <v>-0.13963</v>
+      </c>
+      <c r="AC20" s="0" t="n">
+        <v>-0.058274</v>
+      </c>
+      <c r="AD20" s="0" t="n">
+        <v>-0.38957</v>
+      </c>
+      <c r="AE20" s="0" t="n">
+        <v>-0.075652</v>
+      </c>
+      <c r="AF20" s="0" t="n">
+        <v>0.14047</v>
+      </c>
+      <c r="AG20" s="0" t="n">
+        <v>-0.029565</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>0.28783</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>-0.47542</v>
+      </c>
+      <c r="V21" s="0" t="n">
+        <v>0.4313</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>-0.32435</v>
+      </c>
+      <c r="X21" s="0" t="n">
+        <v>-0.36522</v>
+      </c>
+      <c r="Y21" s="0" t="n">
+        <v>-0.6397</v>
+      </c>
+      <c r="Z21" s="0" t="n">
+        <v>0.1035</v>
+      </c>
+      <c r="AA21" s="0" t="n">
+        <v>-0.19043</v>
+      </c>
+      <c r="AB21" s="0" t="n">
+        <v>-0.10918</v>
+      </c>
+      <c r="AC21" s="0" t="n">
+        <v>-0.42748</v>
+      </c>
+      <c r="AD21" s="0" t="n">
+        <v>-0.18609</v>
+      </c>
+      <c r="AE21" s="0" t="n">
+        <v>-0.3687</v>
+      </c>
+      <c r="AF21" s="0" t="n">
+        <v>-0.12264</v>
+      </c>
+      <c r="AG21" s="0" t="n">
+        <v>0.18957</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <v>0.11396</v>
+      </c>
+      <c r="V22" s="0" t="n">
+        <v>0.067826</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <v>-0.056522</v>
+      </c>
+      <c r="X22" s="0" t="n">
+        <v>-0.1313</v>
+      </c>
+      <c r="Y22" s="0" t="n">
+        <v>0.1583</v>
+      </c>
+      <c r="Z22" s="0" t="n">
+        <v>0.26614</v>
+      </c>
+      <c r="AA22" s="0" t="n">
+        <v>-0.2087</v>
+      </c>
+      <c r="AB22" s="0" t="n">
+        <v>-0.2575</v>
+      </c>
+      <c r="AC22" s="0" t="n">
+        <v>-0.052185</v>
+      </c>
+      <c r="AD22" s="0" t="n">
+        <v>-0.12348</v>
+      </c>
+      <c r="AE22" s="0" t="n">
+        <v>-0.33913</v>
+      </c>
+      <c r="AF22" s="0" t="n">
+        <v>-0.24092</v>
+      </c>
+      <c r="AG22" s="0" t="n">
+        <v>-0.033043</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V23" s="0" t="n">
+        <v>-0.44019</v>
+      </c>
+      <c r="W23" s="0" t="n">
+        <v>-0.014789</v>
+      </c>
+      <c r="X23" s="0" t="n">
+        <v>0.064811</v>
+      </c>
+      <c r="Y23" s="0" t="n">
+        <v>0.88928</v>
+      </c>
+      <c r="Z23" s="0" t="n">
+        <v>0.40113</v>
+      </c>
+      <c r="AA23" s="0" t="n">
+        <v>0.13397</v>
+      </c>
+      <c r="AB23" s="0" t="n">
+        <v>0.33333</v>
+      </c>
+      <c r="AC23" s="0" t="n">
+        <v>0.61475</v>
+      </c>
+      <c r="AD23" s="0" t="n">
+        <v>0.22749</v>
+      </c>
+      <c r="AE23" s="0" t="n">
+        <v>0.21096</v>
+      </c>
+      <c r="AF23" s="0" t="n">
+        <v>0.19534</v>
+      </c>
+      <c r="AG23" s="0" t="n">
+        <v>0.0095694</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W24" s="0" t="n">
+        <v>-0.064348</v>
+      </c>
+      <c r="X24" s="0" t="n">
+        <v>-0.10609</v>
+      </c>
+      <c r="Y24" s="0" t="n">
+        <v>-0.48837</v>
+      </c>
+      <c r="Z24" s="0" t="n">
+        <v>-0.2918</v>
+      </c>
+      <c r="AA24" s="0" t="n">
+        <v>-0.32696</v>
+      </c>
+      <c r="AB24" s="0" t="n">
+        <v>-0.26359</v>
+      </c>
+      <c r="AC24" s="0" t="n">
+        <v>-0.57273</v>
+      </c>
+      <c r="AD24" s="0" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="AE24" s="0" t="n">
+        <v>-0.090435</v>
+      </c>
+      <c r="AF24" s="0" t="n">
+        <v>-0.20222</v>
+      </c>
+      <c r="AG24" s="0" t="n">
+        <v>-0.3087</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X25" s="0" t="n">
+        <v>-0.036522</v>
+      </c>
+      <c r="Y25" s="0" t="n">
+        <v>0.21092</v>
+      </c>
+      <c r="Z25" s="0" t="n">
+        <v>0.022179</v>
+      </c>
+      <c r="AA25" s="0" t="n">
+        <v>0.39478</v>
+      </c>
+      <c r="AB25" s="0" t="n">
+        <v>0.10091</v>
+      </c>
+      <c r="AC25" s="0" t="n">
+        <v>0.23353</v>
+      </c>
+      <c r="AD25" s="0" t="n">
+        <v>0.24957</v>
+      </c>
+      <c r="AE25" s="0" t="n">
+        <v>0.064348</v>
+      </c>
+      <c r="AF25" s="0" t="n">
+        <v>-0.197</v>
+      </c>
+      <c r="AG25" s="0" t="n">
+        <v>-0.11217</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y26" s="0" t="n">
+        <v>0.17917</v>
+      </c>
+      <c r="Z26" s="0" t="n">
+        <v>-0.25701</v>
+      </c>
+      <c r="AA26" s="0" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="AB26" s="0" t="n">
+        <v>0.018704</v>
+      </c>
+      <c r="AC26" s="0" t="n">
+        <v>0.0043488</v>
+      </c>
+      <c r="AD26" s="0" t="n">
+        <v>-0.17652</v>
+      </c>
+      <c r="AE26" s="0" t="n">
+        <v>0.57826</v>
+      </c>
+      <c r="AF26" s="0" t="n">
+        <v>0.16395</v>
+      </c>
+      <c r="AG26" s="0" t="n">
+        <v>-0.17652</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z27" s="0" t="n">
+        <v>0.19226</v>
+      </c>
+      <c r="AA27" s="0" t="n">
+        <v>0.12611</v>
+      </c>
+      <c r="AB27" s="0" t="n">
+        <v>0.2419</v>
+      </c>
+      <c r="AC27" s="0" t="n">
+        <v>0.57721</v>
+      </c>
+      <c r="AD27" s="0" t="n">
+        <v>0.16351</v>
+      </c>
+      <c r="AE27" s="0" t="n">
+        <v>0.34964</v>
+      </c>
+      <c r="AF27" s="0" t="n">
+        <v>0.15355</v>
+      </c>
+      <c r="AG27" s="0" t="n">
+        <v>-0.1683</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA28" s="0" t="n">
+        <v>0.090454</v>
+      </c>
+      <c r="AB28" s="0" t="n">
+        <v>0.081792</v>
+      </c>
+      <c r="AC28" s="0" t="n">
+        <v>0.3371</v>
+      </c>
+      <c r="AD28" s="0" t="n">
+        <v>0.27963</v>
+      </c>
+      <c r="AE28" s="0" t="n">
+        <v>-0.43357</v>
+      </c>
+      <c r="AF28" s="0" t="n">
+        <v>0.18312</v>
+      </c>
+      <c r="AG28" s="0" t="n">
+        <v>0.32311</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB29" s="0" t="n">
+        <v>0.58547</v>
+      </c>
+      <c r="AC29" s="0" t="n">
+        <v>0.46097</v>
+      </c>
+      <c r="AD29" s="0" t="n">
+        <v>0.52087</v>
+      </c>
+      <c r="AE29" s="0" t="n">
+        <v>0.34261</v>
+      </c>
+      <c r="AF29" s="0" t="n">
+        <v>-0.020874</v>
+      </c>
+      <c r="AG29" s="0" t="n">
+        <v>0.37913</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC30" s="0" t="n">
+        <v>0.66087</v>
+      </c>
+      <c r="AD30" s="0" t="n">
+        <v>0.53545</v>
+      </c>
+      <c r="AE30" s="0" t="n">
+        <v>0.36146</v>
+      </c>
+      <c r="AF30" s="0" t="n">
+        <v>0.03089</v>
+      </c>
+      <c r="AG30" s="0" t="n">
+        <v>0.45237</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD31" s="0" t="n">
+        <v>0.50707</v>
+      </c>
+      <c r="AE31" s="0" t="n">
+        <v>0.29137</v>
+      </c>
+      <c r="AF31" s="0" t="n">
+        <v>-0.077425</v>
+      </c>
+      <c r="AG31" s="0" t="n">
+        <v>0.22048</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE32" s="0" t="n">
+        <v>0.047826</v>
+      </c>
+      <c r="AF32" s="0" t="n">
+        <v>0.17439</v>
+      </c>
+      <c r="AG32" s="0" t="n">
+        <v>0.1487</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF33" s="0" t="n">
+        <v>0.0047836</v>
+      </c>
+      <c r="AG33" s="0" t="n">
+        <v>-0.18783</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG34" s="0" t="n">
+        <v>0.028267</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AG1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E4:AG33">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>